<commit_message>
Latest update code for Product InvenotryItem
</commit_message>
<xml_diff>
--- a/TestData/Excel-Files/Lead_Add Imports_With Default Fileds 1.1.xlsx
+++ b/TestData/Excel-Files/Lead_Add Imports_With Default Fileds 1.1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6137" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8057" uniqueCount="627">
   <si>
     <t>Title</t>
   </si>
@@ -1524,6 +1524,378 @@
   </si>
   <si>
     <t>30896</t>
+  </si>
+  <si>
+    <t>Kevin189</t>
+  </si>
+  <si>
+    <t>Alexander998</t>
+  </si>
+  <si>
+    <t>Wright671</t>
+  </si>
+  <si>
+    <t>import396@lionobytes.com</t>
+  </si>
+  <si>
+    <t>7030205326</t>
+  </si>
+  <si>
+    <t>25898681</t>
+  </si>
+  <si>
+    <t>2550803</t>
+  </si>
+  <si>
+    <t>lead146@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628367</t>
+  </si>
+  <si>
+    <t>20497</t>
+  </si>
+  <si>
+    <t>30446</t>
+  </si>
+  <si>
+    <t>Note Added 1937</t>
+  </si>
+  <si>
+    <t>Kevin826</t>
+  </si>
+  <si>
+    <t>Alexander286</t>
+  </si>
+  <si>
+    <t>Wright686</t>
+  </si>
+  <si>
+    <t>import325@lionobytes.com</t>
+  </si>
+  <si>
+    <t>7030205897</t>
+  </si>
+  <si>
+    <t>25898086</t>
+  </si>
+  <si>
+    <t>DBA1038</t>
+  </si>
+  <si>
+    <t>2550967</t>
+  </si>
+  <si>
+    <t>lead815@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628071</t>
+  </si>
+  <si>
+    <t>20872</t>
+  </si>
+  <si>
+    <t>30717</t>
+  </si>
+  <si>
+    <t>Note Added 1518</t>
+  </si>
+  <si>
+    <t>Alexander516</t>
+  </si>
+  <si>
+    <t>Wright652</t>
+  </si>
+  <si>
+    <t>import429@lionobytes.com</t>
+  </si>
+  <si>
+    <t>7030205460</t>
+  </si>
+  <si>
+    <t>25898895</t>
+  </si>
+  <si>
+    <t>DBA1328</t>
+  </si>
+  <si>
+    <t>2550484</t>
+  </si>
+  <si>
+    <t>lead160@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628606</t>
+  </si>
+  <si>
+    <t>20669</t>
+  </si>
+  <si>
+    <t>30706</t>
+  </si>
+  <si>
+    <t>Note Added 1615</t>
+  </si>
+  <si>
+    <t>Alexander375</t>
+  </si>
+  <si>
+    <t>Wright463</t>
+  </si>
+  <si>
+    <t>import042@lionobytes.com</t>
+  </si>
+  <si>
+    <t>7030205379</t>
+  </si>
+  <si>
+    <t>25898435</t>
+  </si>
+  <si>
+    <t>DBA1874</t>
+  </si>
+  <si>
+    <t>2550585</t>
+  </si>
+  <si>
+    <t>lead060@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628669</t>
+  </si>
+  <si>
+    <t>20493</t>
+  </si>
+  <si>
+    <t>30540</t>
+  </si>
+  <si>
+    <t>Note Added 1485</t>
+  </si>
+  <si>
+    <t>Kevin539</t>
+  </si>
+  <si>
+    <t>Alexander379</t>
+  </si>
+  <si>
+    <t>Wright310</t>
+  </si>
+  <si>
+    <t>import897@lionobytes.com</t>
+  </si>
+  <si>
+    <t>7030205971</t>
+  </si>
+  <si>
+    <t>25898941</t>
+  </si>
+  <si>
+    <t>2550260</t>
+  </si>
+  <si>
+    <t>lead150@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628278</t>
+  </si>
+  <si>
+    <t>20574</t>
+  </si>
+  <si>
+    <t>30629</t>
+  </si>
+  <si>
+    <t>Note Added 1386</t>
+  </si>
+  <si>
+    <t>Kevin885</t>
+  </si>
+  <si>
+    <t>Alexander669</t>
+  </si>
+  <si>
+    <t>Wright273</t>
+  </si>
+  <si>
+    <t>import211@lionobytes.com</t>
+  </si>
+  <si>
+    <t>7030205974</t>
+  </si>
+  <si>
+    <t>25898043</t>
+  </si>
+  <si>
+    <t>DBA1041</t>
+  </si>
+  <si>
+    <t>2550412</t>
+  </si>
+  <si>
+    <t>lead106@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628168</t>
+  </si>
+  <si>
+    <t>20777</t>
+  </si>
+  <si>
+    <t>30885</t>
+  </si>
+  <si>
+    <t>Note Added 1309</t>
+  </si>
+  <si>
+    <t>Kevin072</t>
+  </si>
+  <si>
+    <t>Alexander814</t>
+  </si>
+  <si>
+    <t>Wright208</t>
+  </si>
+  <si>
+    <t>import880@lionobytes.com</t>
+  </si>
+  <si>
+    <t>7030205765</t>
+  </si>
+  <si>
+    <t>25898718</t>
+  </si>
+  <si>
+    <t>DBA1653</t>
+  </si>
+  <si>
+    <t>2550101</t>
+  </si>
+  <si>
+    <t>lead262@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628886</t>
+  </si>
+  <si>
+    <t>20879</t>
+  </si>
+  <si>
+    <t>30268</t>
+  </si>
+  <si>
+    <t>Note Added 1287</t>
+  </si>
+  <si>
+    <t>Kevin069</t>
+  </si>
+  <si>
+    <t>Alexander657</t>
+  </si>
+  <si>
+    <t>Wright588</t>
+  </si>
+  <si>
+    <t>import155@lionobytes.com</t>
+  </si>
+  <si>
+    <t>7030205640</t>
+  </si>
+  <si>
+    <t>25898661</t>
+  </si>
+  <si>
+    <t>DBA1081</t>
+  </si>
+  <si>
+    <t>2550087</t>
+  </si>
+  <si>
+    <t>lead368@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628123</t>
+  </si>
+  <si>
+    <t>20540</t>
+  </si>
+  <si>
+    <t>30567</t>
+  </si>
+  <si>
+    <t>Note Added 1557</t>
+  </si>
+  <si>
+    <t>Kevin834</t>
+  </si>
+  <si>
+    <t>Alexander400</t>
+  </si>
+  <si>
+    <t>Wright548</t>
+  </si>
+  <si>
+    <t>import568@lionobytes.com</t>
+  </si>
+  <si>
+    <t>25898932</t>
+  </si>
+  <si>
+    <t>DBA1251</t>
+  </si>
+  <si>
+    <t>2550923</t>
+  </si>
+  <si>
+    <t>lead200@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628324</t>
+  </si>
+  <si>
+    <t>20125</t>
+  </si>
+  <si>
+    <t>30788</t>
+  </si>
+  <si>
+    <t>Note Added 1631</t>
+  </si>
+  <si>
+    <t>Kevin176</t>
+  </si>
+  <si>
+    <t>Alexander007</t>
+  </si>
+  <si>
+    <t>Wright546</t>
+  </si>
+  <si>
+    <t>import546@lionobytes.com</t>
+  </si>
+  <si>
+    <t>7030205590</t>
+  </si>
+  <si>
+    <t>25898771</t>
+  </si>
+  <si>
+    <t>DBA1595</t>
+  </si>
+  <si>
+    <t>2550187</t>
+  </si>
+  <si>
+    <t>lead906@lionobytes.com</t>
+  </si>
+  <si>
+    <t>9075628499</t>
+  </si>
+  <si>
+    <t>20972</t>
+  </si>
+  <si>
+    <t>Note Added 1417</t>
   </si>
 </sst>
 </file>
@@ -2100,972 +2472,972 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="B2" t="s">
-        <v>441</v>
-      </c>
-      <c r="C2" t="s">
-        <v>442</v>
-      </c>
-      <c r="D2" t="s">
-        <v>443</v>
-      </c>
-      <c r="E2" t="s">
-        <v>444</v>
-      </c>
-      <c r="F2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>445</v>
-      </c>
-      <c r="J2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>53</v>
-      </c>
-      <c r="R2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="B2" t="s" s="0">
+        <v>564</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>565</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>566</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>567</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>568</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="Q2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="S2" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="T2" t="s">
-        <v>53</v>
-      </c>
-      <c r="U2" t="s">
-        <v>53</v>
-      </c>
-      <c r="V2" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="T2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="U2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="V2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="W2" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="X2" t="s">
-        <v>446</v>
-      </c>
-      <c r="Y2" t="s">
+      <c r="X2" t="s" s="0">
+        <v>569</v>
+      </c>
+      <c r="Y2" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="Z2" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="AB2" t="s">
-        <v>447</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>448</v>
-      </c>
-      <c r="AD2" t="s">
+      <c r="AB2" t="s" s="0">
+        <v>570</v>
+      </c>
+      <c r="AC2" t="s" s="0">
+        <v>571</v>
+      </c>
+      <c r="AD2" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AG2" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AH2" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AI2" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>449</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>450</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>451</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>452</v>
-      </c>
-      <c r="AS2" t="s">
+      <c r="AJ2" t="s" s="0">
+        <v>572</v>
+      </c>
+      <c r="AK2" t="s" s="0">
+        <v>573</v>
+      </c>
+      <c r="AL2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AM2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AN2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AO2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AP2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AQ2" t="s" s="0">
+        <v>574</v>
+      </c>
+      <c r="AR2" t="s" s="0">
+        <v>575</v>
+      </c>
+      <c r="AS2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AT2" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AU2" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="AV2" t="s">
-        <v>453</v>
-      </c>
-      <c r="AW2" t="s">
+      <c r="AV2" t="s" s="0">
+        <v>576</v>
+      </c>
+      <c r="AW2" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AX2" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="AY2" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="AZ2" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BA2" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BB2" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BC2" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BD2" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="BE2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL2" t="s">
+      <c r="BE2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BF2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BG2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BH2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BI2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BJ2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BK2" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BL2" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="B3" t="s">
-        <v>454</v>
-      </c>
-      <c r="C3" t="s">
-        <v>455</v>
-      </c>
-      <c r="D3" t="s">
-        <v>456</v>
-      </c>
-      <c r="E3" t="s">
-        <v>457</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" t="s">
-        <v>331</v>
-      </c>
-      <c r="J3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" t="s">
-        <v>53</v>
-      </c>
-      <c r="L3" t="s">
-        <v>53</v>
-      </c>
-      <c r="M3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N3" t="s">
-        <v>53</v>
-      </c>
-      <c r="O3" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>53</v>
-      </c>
-      <c r="R3" t="s">
-        <v>53</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>577</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>578</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>579</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>580</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>581</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="P3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="Q3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="R3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="S3" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="T3" t="s">
-        <v>53</v>
-      </c>
-      <c r="U3" t="s">
-        <v>53</v>
-      </c>
-      <c r="V3" t="s">
-        <v>53</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="T3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="U3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="V3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="W3" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="X3" t="s">
-        <v>458</v>
-      </c>
-      <c r="Y3" t="s">
+      <c r="X3" t="s" s="0">
+        <v>582</v>
+      </c>
+      <c r="Y3" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="AB3" t="s">
-        <v>459</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>460</v>
-      </c>
-      <c r="AD3" t="s">
+      <c r="AB3" t="s" s="0">
+        <v>583</v>
+      </c>
+      <c r="AC3" t="s" s="0">
+        <v>584</v>
+      </c>
+      <c r="AD3" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AE3" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AF3" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AG3" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AH3" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AI3" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="AJ3" t="s">
-        <v>461</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>462</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>463</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>464</v>
-      </c>
-      <c r="AS3" t="s">
+      <c r="AJ3" t="s" s="0">
+        <v>585</v>
+      </c>
+      <c r="AK3" t="s" s="0">
+        <v>586</v>
+      </c>
+      <c r="AL3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AM3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AN3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AO3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AP3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AQ3" t="s" s="0">
+        <v>587</v>
+      </c>
+      <c r="AR3" t="s" s="0">
+        <v>588</v>
+      </c>
+      <c r="AS3" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AT3" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="AU3" t="s">
+      <c r="AU3" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="AV3" t="s">
-        <v>465</v>
-      </c>
-      <c r="AW3" t="s">
+      <c r="AV3" t="s" s="0">
+        <v>589</v>
+      </c>
+      <c r="AW3" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="AX3" t="s">
+      <c r="AX3" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="AY3" t="s">
+      <c r="AY3" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="AZ3" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BA3" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BB3" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="BC3" t="s">
+      <c r="BC3" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="BD3" t="s">
+      <c r="BD3" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="BE3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BH3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BI3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BK3" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL3" t="s">
+      <c r="BE3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BF3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BG3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BH3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BI3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BJ3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BK3" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BL3" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="B4" t="s">
-        <v>466</v>
-      </c>
-      <c r="C4" t="s">
-        <v>467</v>
-      </c>
-      <c r="D4" t="s">
-        <v>468</v>
-      </c>
-      <c r="E4" t="s">
-        <v>469</v>
-      </c>
-      <c r="F4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" t="s">
-        <v>470</v>
-      </c>
-      <c r="J4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" t="s">
-        <v>53</v>
-      </c>
-      <c r="O4" t="s">
-        <v>53</v>
-      </c>
-      <c r="P4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>53</v>
-      </c>
-      <c r="R4" t="s">
-        <v>53</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>590</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>591</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>592</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>593</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>594</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="P4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="Q4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="R4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="S4" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="T4" t="s">
-        <v>53</v>
-      </c>
-      <c r="U4" t="s">
-        <v>53</v>
-      </c>
-      <c r="V4" t="s">
-        <v>53</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="T4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="U4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="V4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="W4" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="X4" t="s">
-        <v>471</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="X4" t="s" s="0">
+        <v>595</v>
+      </c>
+      <c r="Y4" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="Z4" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AA4" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="AB4" t="s">
-        <v>472</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>473</v>
-      </c>
-      <c r="AD4" t="s">
+      <c r="AB4" t="s" s="0">
+        <v>596</v>
+      </c>
+      <c r="AC4" t="s" s="0">
+        <v>597</v>
+      </c>
+      <c r="AD4" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AE4" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AF4" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AG4" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AH4" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AI4" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="AJ4" t="s">
-        <v>474</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>475</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>476</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>262</v>
-      </c>
-      <c r="AS4" t="s">
+      <c r="AJ4" t="s" s="0">
+        <v>598</v>
+      </c>
+      <c r="AK4" t="s" s="0">
+        <v>599</v>
+      </c>
+      <c r="AL4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AM4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AN4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AO4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AP4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AQ4" t="s" s="0">
+        <v>600</v>
+      </c>
+      <c r="AR4" t="s" s="0">
+        <v>601</v>
+      </c>
+      <c r="AS4" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AT4" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="AU4" t="s">
+      <c r="AU4" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="AV4" t="s">
-        <v>477</v>
-      </c>
-      <c r="AW4" t="s">
+      <c r="AV4" t="s" s="0">
+        <v>602</v>
+      </c>
+      <c r="AW4" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="AX4" t="s">
+      <c r="AX4" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="AY4" t="s">
+      <c r="AY4" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="AZ4" t="s">
+      <c r="AZ4" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="BA4" t="s">
+      <c r="BA4" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="BB4" t="s">
+      <c r="BB4" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="BC4" t="s">
+      <c r="BC4" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="BD4" t="s">
+      <c r="BD4" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="BE4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BG4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BH4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BI4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BJ4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BK4" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL4" t="s">
+      <c r="BE4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BF4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BG4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BH4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BI4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BJ4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BK4" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BL4" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="B5" t="s">
-        <v>478</v>
-      </c>
-      <c r="C5" t="s">
-        <v>479</v>
-      </c>
-      <c r="D5" t="s">
-        <v>480</v>
-      </c>
-      <c r="E5" t="s">
-        <v>481</v>
-      </c>
-      <c r="F5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" t="s">
-        <v>482</v>
-      </c>
-      <c r="J5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" t="s">
-        <v>53</v>
-      </c>
-      <c r="L5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" t="s">
-        <v>53</v>
-      </c>
-      <c r="N5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" t="s">
-        <v>53</v>
-      </c>
-      <c r="P5" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>53</v>
-      </c>
-      <c r="R5" t="s">
-        <v>53</v>
-      </c>
-      <c r="S5" t="s">
+      <c r="B5" t="s" s="0">
+        <v>603</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>604</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>605</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>606</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>294</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="L5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="M5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="N5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="O5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="P5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="Q5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="R5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="S5" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="T5" t="s">
-        <v>53</v>
-      </c>
-      <c r="U5" t="s">
-        <v>53</v>
-      </c>
-      <c r="V5" t="s">
-        <v>53</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="T5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="U5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="V5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="W5" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="X5" t="s">
-        <v>483</v>
-      </c>
-      <c r="Y5" t="s">
+      <c r="X5" t="s" s="0">
+        <v>607</v>
+      </c>
+      <c r="Y5" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="Z5" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AA5" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="AB5" t="s">
-        <v>484</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>485</v>
-      </c>
-      <c r="AD5" t="s">
+      <c r="AB5" t="s" s="0">
+        <v>608</v>
+      </c>
+      <c r="AC5" t="s" s="0">
+        <v>609</v>
+      </c>
+      <c r="AD5" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AE5" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="AF5" t="s">
+      <c r="AF5" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="AG5" t="s">
+      <c r="AG5" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AH5" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="AI5" t="s">
+      <c r="AI5" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="AJ5" t="s">
-        <v>486</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>487</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ5" t="s">
-        <v>488</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>489</v>
-      </c>
-      <c r="AS5" t="s">
+      <c r="AJ5" t="s" s="0">
+        <v>610</v>
+      </c>
+      <c r="AK5" t="s" s="0">
+        <v>611</v>
+      </c>
+      <c r="AL5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AM5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AN5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AO5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AP5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AQ5" t="s" s="0">
+        <v>612</v>
+      </c>
+      <c r="AR5" t="s" s="0">
+        <v>613</v>
+      </c>
+      <c r="AS5" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AT5" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="AU5" t="s">
+      <c r="AU5" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="AV5" t="s">
-        <v>490</v>
-      </c>
-      <c r="AW5" t="s">
+      <c r="AV5" t="s" s="0">
+        <v>614</v>
+      </c>
+      <c r="AW5" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="AX5" t="s">
+      <c r="AX5" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="AY5" t="s">
+      <c r="AY5" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="AZ5" t="s">
+      <c r="AZ5" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="BA5" t="s">
+      <c r="BA5" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="BB5" t="s">
+      <c r="BB5" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="BC5" t="s">
+      <c r="BC5" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="BD5" t="s">
+      <c r="BD5" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="BE5" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF5" t="s">
-        <v>53</v>
-      </c>
-      <c r="BG5" t="s">
-        <v>53</v>
-      </c>
-      <c r="BH5" t="s">
-        <v>53</v>
-      </c>
-      <c r="BI5" t="s">
-        <v>53</v>
-      </c>
-      <c r="BJ5" t="s">
-        <v>53</v>
-      </c>
-      <c r="BK5" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL5" t="s">
+      <c r="BE5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BF5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BG5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BH5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BI5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BJ5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BK5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BL5" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>250</v>
       </c>
-      <c r="B6" t="s">
-        <v>491</v>
-      </c>
-      <c r="C6" t="s">
-        <v>492</v>
-      </c>
-      <c r="D6" t="s">
-        <v>493</v>
-      </c>
-      <c r="E6" t="s">
-        <v>494</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" t="s">
-        <v>495</v>
-      </c>
-      <c r="J6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" t="s">
-        <v>53</v>
-      </c>
-      <c r="L6" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" t="s">
-        <v>53</v>
-      </c>
-      <c r="O6" t="s">
-        <v>53</v>
-      </c>
-      <c r="P6" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>53</v>
-      </c>
-      <c r="R6" t="s">
-        <v>53</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="B6" t="s" s="0">
+        <v>615</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>616</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>617</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>618</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>619</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="Q6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="R6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="S6" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="T6" t="s">
-        <v>53</v>
-      </c>
-      <c r="U6" t="s">
-        <v>53</v>
-      </c>
-      <c r="V6" t="s">
-        <v>53</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="T6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="U6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="V6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="W6" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="X6" t="s">
-        <v>496</v>
-      </c>
-      <c r="Y6" t="s">
+      <c r="X6" t="s" s="0">
+        <v>620</v>
+      </c>
+      <c r="Y6" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="Z6" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AA6" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="AB6" t="s">
-        <v>497</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>498</v>
-      </c>
-      <c r="AD6" t="s">
+      <c r="AB6" t="s" s="0">
+        <v>621</v>
+      </c>
+      <c r="AC6" t="s" s="0">
+        <v>622</v>
+      </c>
+      <c r="AD6" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AE6" t="s" s="0">
         <v>59</v>
       </c>
-      <c r="AF6" t="s">
+      <c r="AF6" t="s" s="0">
         <v>60</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AG6" t="s" s="0">
         <v>61</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AH6" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="AI6" t="s">
+      <c r="AI6" t="s" s="0">
         <v>63</v>
       </c>
-      <c r="AJ6" t="s">
-        <v>499</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>500</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AM6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AN6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AO6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AP6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ6" t="s">
-        <v>501</v>
-      </c>
-      <c r="AR6" t="s">
-        <v>502</v>
-      </c>
-      <c r="AS6" t="s">
+      <c r="AJ6" t="s" s="0">
+        <v>623</v>
+      </c>
+      <c r="AK6" t="s" s="0">
+        <v>624</v>
+      </c>
+      <c r="AL6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AM6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AN6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AO6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AP6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="AQ6" t="s" s="0">
+        <v>625</v>
+      </c>
+      <c r="AR6" t="s" s="0">
+        <v>248</v>
+      </c>
+      <c r="AS6" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AT6" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="AU6" t="s">
+      <c r="AU6" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="AV6" t="s">
-        <v>187</v>
-      </c>
-      <c r="AW6" t="s">
+      <c r="AV6" t="s" s="0">
+        <v>626</v>
+      </c>
+      <c r="AW6" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="AX6" t="s">
+      <c r="AX6" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="AY6" t="s">
+      <c r="AY6" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="AZ6" t="s">
+      <c r="AZ6" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="BA6" t="s">
+      <c r="BA6" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="BB6" t="s">
+      <c r="BB6" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="BC6" t="s">
+      <c r="BC6" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="BD6" t="s">
+      <c r="BD6" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="BE6" t="s">
-        <v>53</v>
-      </c>
-      <c r="BF6" t="s">
-        <v>53</v>
-      </c>
-      <c r="BG6" t="s">
-        <v>53</v>
-      </c>
-      <c r="BH6" t="s">
-        <v>53</v>
-      </c>
-      <c r="BI6" t="s">
-        <v>53</v>
-      </c>
-      <c r="BJ6" t="s">
-        <v>53</v>
-      </c>
-      <c r="BK6" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL6" t="s">
+      <c r="BE6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BF6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BG6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BH6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BI6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BJ6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BK6" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="BL6" t="s" s="0">
         <v>53</v>
       </c>
     </row>

</xml_diff>